<commit_message>
text boxes for currents
</commit_message>
<xml_diff>
--- a/GE_Lighting_AlignProjectData.xlsx
+++ b/GE_Lighting_AlignProjectData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmcra\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\Documents\MATLAB\GE Project Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23028" windowHeight="8796"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12360" windowHeight="5664"/>
   </bookViews>
   <sheets>
     <sheet name="LED Spectra" sheetId="1" r:id="rId1"/>
@@ -3780,20 +3780,20 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.15625" style="1"/>
-    <col min="2" max="2" width="11.68359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.68359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16" width="9.15625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16" width="9.109375" style="1"/>
     <col min="17" max="17" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.15625" style="1"/>
+    <col min="18" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:22" x14ac:dyDescent="0.3">
       <c r="C1" s="10" t="s">
         <v>9</v>
       </c>
@@ -3801,7 +3801,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>400</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>3.9100000000000002E-5</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>405</v>
       </c>
@@ -3873,7 +3873,7 @@
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>410</v>
       </c>
@@ -3894,7 +3894,7 @@
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>415</v>
       </c>
@@ -3915,7 +3915,7 @@
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>420</v>
       </c>
@@ -3936,7 +3936,7 @@
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>425</v>
       </c>
@@ -3953,7 +3953,7 @@
         <v>8.7799999999999998E-4</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>430</v>
       </c>
@@ -3970,7 +3970,7 @@
         <v>1.6800000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>435</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>2.8900000000000002E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>440</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>4.5199999999999997E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>445</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>7.0400000000000003E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>450</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>1.0699999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>455</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>1.41E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>460</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>1.3299999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>465</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>470</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>7.8600000000000007E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>475</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>6.62E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>480</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>5.4099999999999999E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
         <v>485</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>4.6100000000000004E-3</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
         <v>490</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>4.3099999999999996E-3</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
         <v>495</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>4.3600000000000002E-3</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
         <v>500</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>4.79E-3</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
         <v>505</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>5.5399999999999998E-3</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
         <v>510</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>6.4599999999999996E-3</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
         <v>515</v>
       </c>
@@ -4259,7 +4259,7 @@
         <v>7.4099999999999999E-3</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="1">
         <v>520</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>8.3599999999999994E-3</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="1">
         <v>525</v>
       </c>
@@ -4293,7 +4293,7 @@
         <v>9.1599999999999997E-3</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="1">
         <v>530</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>9.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" s="1">
         <v>535</v>
       </c>
@@ -4327,7 +4327,7 @@
         <v>1.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" s="1">
         <v>540</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="1">
         <v>545</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>1.14E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="1">
         <v>550</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="1">
         <v>555</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="1">
         <v>560</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>1.24E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="1">
         <v>565</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>1.2699999999999999E-2</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="1">
         <v>570</v>
       </c>
@@ -4446,7 +4446,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="1">
         <v>575</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>1.32E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="1">
         <v>580</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>1.3299999999999999E-2</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="1">
         <v>585</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>1.34E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="1">
         <v>590</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>1.34E-2</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="1">
         <v>595</v>
       </c>
@@ -4531,7 +4531,7 @@
         <v>1.34E-2</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" s="1">
         <v>600</v>
       </c>
@@ -4548,7 +4548,7 @@
         <v>1.32E-2</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" s="1">
         <v>605</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" s="1">
         <v>610</v>
       </c>
@@ -4582,7 +4582,7 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" s="1">
         <v>615</v>
       </c>
@@ -4599,7 +4599,7 @@
         <v>1.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" s="1">
         <v>620</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>1.1599999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" s="1">
         <v>625</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" s="1">
         <v>630</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>1.04E-2</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" s="1">
         <v>635</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>9.75E-3</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52" s="1">
         <v>640</v>
       </c>
@@ -4684,7 +4684,7 @@
         <v>9.0299999999999998E-3</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" s="1">
         <v>645</v>
       </c>
@@ -4701,7 +4701,7 @@
         <v>8.3099999999999997E-3</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" s="1">
         <v>650</v>
       </c>
@@ -4718,7 +4718,7 @@
         <v>7.5799999999999999E-3</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" s="1">
         <v>655</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>6.9199999999999999E-3</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B56" s="1">
         <v>660</v>
       </c>
@@ -4752,7 +4752,7 @@
         <v>6.2300000000000003E-3</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" s="1">
         <v>665</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>5.6299999999999996E-3</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" s="1">
         <v>670</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>5.0600000000000003E-3</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B59" s="1">
         <v>675</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>4.4900000000000001E-3</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" s="1">
         <v>680</v>
       </c>
@@ -4820,7 +4820,7 @@
         <v>3.9699999999999996E-3</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B61" s="1">
         <v>685</v>
       </c>
@@ -4837,7 +4837,7 @@
         <v>3.5300000000000002E-3</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62" s="1">
         <v>690</v>
       </c>
@@ -4854,7 +4854,7 @@
         <v>3.0899999999999999E-3</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63" s="1">
         <v>695</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>2.7299999999999998E-3</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B64" s="1">
         <v>700</v>
       </c>
@@ -4906,20 +4906,20 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.68359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.15625" style="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C1" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="2:5" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4933,12 +4933,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>400</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>6.7850010000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>405</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>0.11020000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>410</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>0.2074</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>415</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>0.37130000000000002</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>420</v>
       </c>
@@ -5008,7 +5008,7 @@
         <v>0.64559999999999995</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>425</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>1.0390501000000001</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>430</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>1.3855999999999999</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>435</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>1.62296</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>440</v>
       </c>
@@ -5064,7 +5064,7 @@
         <v>1.7470600000000001</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>445</v>
       </c>
@@ -5078,7 +5078,7 @@
         <v>1.7826</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>450</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>1.7721100000000001</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>455</v>
       </c>
@@ -5106,7 +5106,7 @@
         <v>1.7441</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>460</v>
       </c>
@@ -5120,7 +5120,7 @@
         <v>1.6692</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>465</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>1.5281</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>470</v>
       </c>
@@ -5148,7 +5148,7 @@
         <v>1.2876399999999999</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>475</v>
       </c>
@@ -5162,7 +5162,7 @@
         <v>1.0419</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>480</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>0.81295010000000001</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
         <v>485</v>
       </c>
@@ -5190,7 +5190,7 @@
         <v>0.61619999999999997</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
         <v>490</v>
       </c>
@@ -5204,7 +5204,7 @@
         <v>0.46517999999999998</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
         <v>495</v>
       </c>
@@ -5218,7 +5218,7 @@
         <v>0.3533</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
         <v>500</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>0.27200000000000002</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
         <v>505</v>
       </c>
@@ -5246,7 +5246,7 @@
         <v>0.21229999999999999</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
         <v>510</v>
       </c>
@@ -5260,7 +5260,7 @@
         <v>0.15820000000000001</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
         <v>515</v>
       </c>
@@ -5274,7 +5274,7 @@
         <v>0.11169999999999999</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="1">
         <v>520</v>
       </c>
@@ -5288,7 +5288,7 @@
         <v>7.8249990000000005E-2</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="1">
         <v>525</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>5.7250009999999997E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="1">
         <v>530</v>
       </c>
@@ -5316,7 +5316,7 @@
         <v>4.2160000000000003E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" s="1">
         <v>535</v>
       </c>
@@ -5330,7 +5330,7 @@
         <v>2.9839999999999998E-2</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" s="1">
         <v>540</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>2.0299999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="1">
         <v>545</v>
       </c>
@@ -5358,7 +5358,7 @@
         <v>1.34E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="1">
         <v>550</v>
       </c>
@@ -5372,7 +5372,7 @@
         <v>8.7499989999999996E-3</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="1">
         <v>555</v>
       </c>
@@ -5386,7 +5386,7 @@
         <v>5.7499990000000004E-3</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="1">
         <v>560</v>
       </c>
@@ -5400,7 +5400,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="1">
         <v>565</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>2.7499989999999999E-3</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="1">
         <v>570</v>
       </c>
@@ -5428,7 +5428,7 @@
         <v>2.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="1">
         <v>575</v>
       </c>
@@ -5442,7 +5442,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="1">
         <v>580</v>
       </c>
@@ -5456,7 +5456,7 @@
         <v>1.6500009999999999E-3</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="1">
         <v>585</v>
       </c>
@@ -5470,7 +5470,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="1">
         <v>590</v>
       </c>
@@ -5484,7 +5484,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" s="1">
         <v>595</v>
       </c>
@@ -5498,7 +5498,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B44" s="1">
         <v>600</v>
       </c>
@@ -5512,7 +5512,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B45" s="1">
         <v>605</v>
       </c>
@@ -5526,7 +5526,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" s="1">
         <v>610</v>
       </c>
@@ -5540,7 +5540,7 @@
         <v>3.4000000000000002E-4</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="1">
         <v>615</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>2.4000000000000001E-4</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" s="1">
         <v>620</v>
       </c>
@@ -5568,7 +5568,7 @@
         <v>1.9000000000000001E-4</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="1">
         <v>625</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" s="1">
         <v>630</v>
       </c>
@@ -5596,7 +5596,7 @@
         <v>4.9999990000000002E-5</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51" s="1">
         <v>635</v>
       </c>
@@ -5610,7 +5610,7 @@
         <v>3.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" s="1">
         <v>640</v>
       </c>
@@ -5624,7 +5624,7 @@
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" s="1">
         <v>645</v>
       </c>
@@ -5638,7 +5638,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" s="1">
         <v>650</v>
       </c>
@@ -5652,7 +5652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B55" s="1">
         <v>655</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B56" s="1">
         <v>660</v>
       </c>
@@ -5680,7 +5680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B57" s="1">
         <v>665</v>
       </c>
@@ -5694,7 +5694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B58" s="1">
         <v>670</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B59" s="1">
         <v>675</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B60" s="1">
         <v>680</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B61" s="1">
         <v>685</v>
       </c>
@@ -5750,7 +5750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B62" s="1">
         <v>690</v>
       </c>
@@ -5764,7 +5764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B63" s="1">
         <v>695</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B64" s="1">
         <v>700</v>
       </c>
@@ -5809,14 +5809,14 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.578125" customWidth="1"/>
-    <col min="3" max="4" width="11.83984375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="4" width="11.88671875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
       <c r="C1" s="11" t="s">
         <v>14</v>
@@ -5826,7 +5826,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="2:5" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
         <v>11</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>12</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>1.3177000000000001</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>13</v>
       </c>

</xml_diff>